<commit_message>
Newest feature code and files
</commit_message>
<xml_diff>
--- a/Manuscript_Code/D_Feature_Comparisons/Output_FeatureComparison/Top1/1concat_filtered_03112025.xlsx
+++ b/Manuscript_Code/D_Feature_Comparisons/Output_FeatureComparison/Top1/1concat_filtered_03112025.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,7 +570,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsCD_Fp</t>
+          <t>franzosa_ControlvsCD_ConvCD</t>
         </is>
       </c>
       <c r="B8">
@@ -580,25 +580,25 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsDisease_Age</t>
+          <t>franzosa_ControlvsCD_Fp</t>
         </is>
       </c>
       <c r="B9">
@@ -608,16 +608,16 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -626,7 +626,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsDisease_ConvDisease</t>
+          <t>franzosa_ControlvsDisease_Age</t>
         </is>
       </c>
       <c r="B10">
@@ -639,26 +639,26 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsDisease_Fp</t>
+          <t>franzosa_ControlvsDisease_ConvDisease</t>
         </is>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -670,23 +670,23 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsUC_Age</t>
+          <t>franzosa_ControlvsDisease_Fp</t>
         </is>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -698,19 +698,19 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>franzosa_ControlvsUC_Fp</t>
+          <t>franzosa_ControlvsUC_Age</t>
         </is>
       </c>
       <c r="B13">
@@ -723,22 +723,22 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>yachida_age</t>
+          <t>franzosa_ControlvsUC_ConvUC</t>
         </is>
       </c>
       <c r="B14">
@@ -751,22 +751,22 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>yachida_alcohol</t>
+          <t>franzosa_ControlvsUC_Fp</t>
         </is>
       </c>
       <c r="B15">
@@ -779,22 +779,22 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>yachida_BrinkmanIndex</t>
+          <t>yachida_age</t>
         </is>
       </c>
       <c r="B16">
@@ -822,7 +822,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>yachida_gender</t>
+          <t>yachida_alcohol</t>
         </is>
       </c>
       <c r="B17">
@@ -835,22 +835,22 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>yachida_healthyvscancer</t>
+          <t>yachida_BrinkmanIndex</t>
         </is>
       </c>
       <c r="B18">
@@ -863,22 +863,22 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>yachida_healthyvsearly</t>
+          <t>yachida_gender</t>
         </is>
       </c>
       <c r="B19">
@@ -906,7 +906,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>yachida_healthyvsstageI_II</t>
+          <t>yachida_healthyvscancer</t>
         </is>
       </c>
       <c r="B20">
@@ -934,7 +934,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>yachida_healthyvsstageIII_IV</t>
+          <t>yachida_healthyvsearly</t>
         </is>
       </c>
       <c r="B21">
@@ -947,22 +947,22 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>wang_age</t>
+          <t>yachida_healthyvsstageI_II</t>
         </is>
       </c>
       <c r="B22">
@@ -975,26 +975,26 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>wang_creatinine</t>
+          <t>yachida_healthyvsstageIII_IV</t>
         </is>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1006,19 +1006,19 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>wang_egfr</t>
+          <t>wang_age</t>
         </is>
       </c>
       <c r="B24">
@@ -1031,26 +1031,26 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>wang_studygroup</t>
+          <t>wang_creatinine</t>
         </is>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1062,40 +1062,96 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>wang_egfr</t>
+        </is>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>wang_studygroup</t>
+        </is>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>wang_urea</t>
         </is>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <v>0</v>
       </c>
     </row>

</xml_diff>